<commit_message>
Increasing the thermometers and histograms sizes by changing the margins, moving and adding titles above the graphs, removing the x-axis for the thermometers, changing the y-axis scale for the histogram, putting the values outside the bars and fixing their display
</commit_message>
<xml_diff>
--- a/dashboard/data/BDD_for_dataviz.xlsx
+++ b/dashboard/data/BDD_for_dataviz.xlsx
@@ -394,13 +394,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -422,11 +426,11 @@
   </sheetPr>
   <dimension ref="A1:AW4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI9" activeCellId="0" sqref="AI9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -574,152 +578,152 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>79</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>87.5</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>93.75</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="C2" s="2" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>62.0610924483549</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="G2" s="2" t="n">
+        <v>0.620610924483549</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>66.4</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="I2" s="2" t="n">
+        <v>0.664</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>72.5</v>
-      </c>
-      <c r="N2" s="0" t="n">
+      <c r="M2" s="2" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="N2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="U2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="X2" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y2" s="2" t="n">
         <v>4.6</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z2" s="2" t="n">
         <v>4.75490196078431</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AA2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AB2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AC2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AD2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AE2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="0" t="s">
+      <c r="AF2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AG2" s="0" t="s">
+      <c r="AG2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AH2" s="0" t="s">
+      <c r="AH2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AI2" s="0" t="s">
+      <c r="AI2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AJ2" s="0" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AK2" s="0" t="s">
+      <c r="AK2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AL2" s="0" t="s">
+      <c r="AL2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AM2" s="0" t="s">
+      <c r="AM2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AN2" s="0" t="n">
+      <c r="AN2" s="2" t="n">
         <v>2327352</v>
       </c>
-      <c r="AO2" s="0" t="n">
+      <c r="AO2" s="2" t="n">
         <v>2019</v>
       </c>
-      <c r="AP2" s="0" t="s">
+      <c r="AP2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AQ2" s="0" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AR2" s="0" t="s">
+      <c r="AR2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AS2" s="0" t="n">
+      <c r="AS2" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="AT2" s="0" t="n">
+      <c r="AT2" s="2" t="n">
         <v>2019</v>
       </c>
-      <c r="AU2" s="0" t="s">
+      <c r="AU2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AV2" s="0" t="n">
+      <c r="AV2" s="2" t="n">
         <v>6.80661464531643</v>
       </c>
-      <c r="AW2" s="0" t="n">
+      <c r="AW2" s="2" t="n">
         <v>5.55147058823529</v>
       </c>
     </row>
@@ -727,148 +731,148 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>83.2</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="C3" s="2" t="n">
+        <v>0.832</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>127.6829940961</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="G3" s="2" t="n">
+        <v>1.276829940961</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>87.4</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>92.5</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>96.25</v>
-      </c>
-      <c r="L3" s="0" t="s">
+      <c r="I3" s="2" t="n">
+        <v>0.874</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0.925</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>0.9625</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="0" t="n">
-        <v>107.5</v>
-      </c>
-      <c r="N3" s="0" t="n">
+      <c r="M3" s="2" t="n">
+        <v>1.075</v>
+      </c>
+      <c r="N3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="U3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3" s="2" t="n">
         <v>5.98039215686275</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="Z3" s="2" t="n">
         <v>4.8468137254902</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AB3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AD3" s="0" t="s">
+      <c r="AD3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AE3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AG3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AH3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AI3" s="0" t="s">
+      <c r="AI3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AJ3" s="0" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AK3" s="0" t="s">
+      <c r="AK3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AL3" s="0" t="s">
+      <c r="AL3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AM3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AN3" s="0" t="n">
+      <c r="AN3" s="2" t="n">
         <v>2327352</v>
       </c>
-      <c r="AO3" s="0" t="n">
+      <c r="AO3" s="2" t="n">
         <v>2019</v>
       </c>
-      <c r="AP3" s="0" t="s">
+      <c r="AP3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AQ3" s="0" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AR3" s="0" t="s">
+      <c r="AR3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AS3" s="0" t="n">
+      <c r="AS3" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="AT3" s="0" t="n">
+      <c r="AT3" s="2" t="n">
         <v>2019</v>
       </c>
-      <c r="AU3" s="0" t="s">
+      <c r="AU3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AV3" s="0" t="n">
+      <c r="AV3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="AW3" s="0" t="n">
+      <c r="AW3" s="2" t="n">
         <v>2.4047619047619</v>
       </c>
     </row>
@@ -876,148 +880,148 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>87.4</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>92.5</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>96.25</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="C4" s="2" t="n">
+        <v>0.874</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.925</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.9625</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>70.2595369</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="G4" s="2" t="n">
+        <v>0.702595369</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>79.84</v>
-      </c>
-      <c r="J4" s="0" t="n">
+      <c r="I4" s="2" t="n">
+        <v>0.7984</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>0.961</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="2" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>4.84243697478992</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="AF4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN4" s="2" t="n">
+        <v>2327352</v>
+      </c>
+      <c r="AO4" s="2" t="n">
+        <v>2019</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS4" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="AT4" s="2" t="n">
+        <v>2020</v>
+      </c>
+      <c r="AU4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>96.1</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="S4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="V4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y4" s="0" t="n">
+      <c r="AV4" s="2" t="n">
         <v>6.99</v>
       </c>
-      <c r="Z4" s="0" t="n">
-        <v>4.84243697478992</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB4" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE4" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF4" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH4" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ4" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK4" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AN4" s="0" t="n">
-        <v>2327352</v>
-      </c>
-      <c r="AO4" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="AP4" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AQ4" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="AR4" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS4" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="AT4" s="0" t="n">
-        <v>2020</v>
-      </c>
-      <c r="AU4" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV4" s="0" t="n">
-        <v>6.99</v>
-      </c>
-      <c r="AW4" s="0" t="n">
+      <c r="AW4" s="2" t="n">
         <v>3.65</v>
       </c>
     </row>

</xml_diff>